<commit_message>
Edit and re export RASD Gantt
</commit_message>
<xml_diff>
--- a/pp/gantt/RASDGantt.xlsx
+++ b/pp/gantt/RASDGantt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Task #</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Davide will start working on this activity in date 05/11/2016</t>
+  </si>
+  <si>
+    <t>Document revision</t>
+  </si>
+  <si>
+    <t>Davide will start working on this activity in date 28/10/2016</t>
   </si>
 </sst>
 </file>
@@ -501,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J1:J21"/>
+      <selection activeCell="C26" sqref="B26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +616,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E19" si="0">CONCATENATE(NETWORKDAYS(F3,G3),"g")</f>
+        <f t="shared" ref="E3:E20" si="0">CONCATENATE(NETWORKDAYS(F3,G3),"g")</f>
         <v>3g</v>
       </c>
       <c r="F3" s="2">
@@ -807,23 +813,20 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>2g</v>
+        <f>CONCATENATE(NETWORKDAYS(F11,G11),"g")</f>
+        <v>3g</v>
       </c>
       <c r="F11" s="2">
-        <v>42670.333333333336</v>
+        <v>42669.333333333336</v>
       </c>
       <c r="G11" s="2">
         <v>42671.666666666664</v>
-      </c>
-      <c r="H11">
-        <v>9</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -840,14 +843,14 @@
         <v>25</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>2g</v>
+        <f>CONCATENATE(NETWORKDAYS(F12,G12),"g")</f>
+        <v>1g</v>
       </c>
       <c r="F12" s="2">
         <v>42670.333333333336</v>
       </c>
       <c r="G12" s="2">
-        <v>42671.666666666664</v>
+        <v>42670.666666666664</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -858,20 +861,26 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>2g</v>
       </c>
       <c r="F13" s="2">
-        <v>42669.333333333336</v>
+        <v>42670.333333333336</v>
       </c>
       <c r="G13" s="2">
         <v>42671.666666666664</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -943,13 +952,13 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>3g</v>
       </c>
       <c r="F16" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="G16" s="2">
-        <v>42687.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -991,13 +1000,13 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>3g</v>
       </c>
       <c r="F18" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="G18" s="2">
-        <v>42685.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -1018,16 +1027,40 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>3g</v>
       </c>
       <c r="F19" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="G19" s="2">
-        <v>42685.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="I19">
         <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>4g</v>
+      </c>
+      <c r="F20" s="2">
+        <v>42682.333333333336</v>
+      </c>
+      <c r="G20" s="2">
+        <v>42685.666666666664</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>